<commit_message>
Export statistic results to csv
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1BDA62-DE7B-4129-976C-AC9F26428FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2A4703-0279-41D7-844E-D8BC400999BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -139,9 +139,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,7 +423,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +555,7 @@
       <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -607,15 +604,24 @@
       <c r="D23" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E23" s="1">
+        <v>0.99080000000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E24" s="1">
+        <v>0.98570000000000002</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.98519999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added list of drug candidates and saving dataset 1 and 2 separately
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2A4703-0279-41D7-844E-D8BC400999BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C910CC-6828-4350-AC06-42FD5AB1F675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -54,9 +54,6 @@
     <t>G1</t>
   </si>
   <si>
-    <t>G2</t>
-  </si>
-  <si>
     <t>hidden dimension</t>
   </si>
   <si>
@@ -94,6 +91,30 @@
   </si>
   <si>
     <t>0.02792497426001874</t>
+  </si>
+  <si>
+    <t>G2 #2</t>
+  </si>
+  <si>
+    <t>G2 #1</t>
+  </si>
+  <si>
+    <t>0.017630062959213853</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>G2 #3</t>
+  </si>
+  <si>
+    <t>0.013477408995651594</t>
+  </si>
+  <si>
+    <t>G2 #4</t>
+  </si>
+  <si>
+    <t>0.00040232263806239127</t>
   </si>
 </sst>
 </file>
@@ -420,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F25"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,22 +453,34 @@
     <col min="4" max="4" width="27.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
@@ -457,8 +490,17 @@
       <c r="F4" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
@@ -468,8 +510,17 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -479,8 +530,17 @@
       <c r="F6" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
@@ -490,8 +550,17 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
@@ -501,8 +570,17 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
@@ -512,15 +590,24 @@
       <c r="F9" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <v>128</v>
+      </c>
+      <c r="H9" s="1">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>64</v>
@@ -528,10 +615,19 @@
       <c r="F14" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <v>256</v>
+      </c>
+      <c r="H14" s="1">
+        <v>256</v>
+      </c>
+      <c r="I14" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1">
         <v>128</v>
@@ -539,8 +635,17 @@
       <c r="F15" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>256</v>
+      </c>
+      <c r="H15" s="1">
+        <v>64</v>
+      </c>
+      <c r="I15" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
@@ -550,32 +655,59 @@
       <c r="F16" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>200</v>
+      </c>
+      <c r="H16" s="1">
+        <v>100</v>
+      </c>
+      <c r="I16" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -583,10 +715,19 @@
       <c r="F19" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -594,34 +735,79 @@
       <c r="F20" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="1">
+        <v>0.99029999999999996</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.95740000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.96150000000000002</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.94650000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="1">
-        <v>0.99080000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.98570000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E25" s="1">
-        <v>0.98519999999999996</v>
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.96419999999999995</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.9758</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.97840000000000005</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.9476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated explanations for dataset 1
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C910CC-6828-4350-AC06-42FD5AB1F675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC4666-CAA2-49DF-A298-CD25003058AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -115,6 +115,36 @@
   </si>
   <si>
     <t>0.00040232263806239127</t>
+  </si>
+  <si>
+    <t>Metapath2Vec</t>
+  </si>
+  <si>
+    <t>epoch_m2v</t>
+  </si>
+  <si>
+    <t>num_walks</t>
+  </si>
+  <si>
+    <t>walk_length</t>
+  </si>
+  <si>
+    <t>context_size</t>
+  </si>
+  <si>
+    <t>dimensions_m2v</t>
+  </si>
+  <si>
+    <t>0.004935371639375551</t>
+  </si>
+  <si>
+    <t>lr_m2v</t>
+  </si>
+  <si>
+    <t>0.08012563751611058</t>
+  </si>
+  <si>
+    <t>G2</t>
   </si>
 </sst>
 </file>
@@ -441,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,14 +486,20 @@
     <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
@@ -479,8 +515,14 @@
       <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
@@ -499,8 +541,14 @@
       <c r="I4" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
@@ -519,8 +567,14 @@
       <c r="I5" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -539,8 +593,14 @@
       <c r="I6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
@@ -559,8 +619,14 @@
       <c r="I7" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
@@ -579,8 +645,14 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
@@ -599,13 +671,29 @@
       <c r="I9" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
@@ -624,8 +712,14 @@
       <c r="I14" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
@@ -644,8 +738,14 @@
       <c r="I15" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
@@ -664,8 +764,14 @@
       <c r="I16" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
@@ -684,8 +790,14 @@
       <c r="I17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
@@ -704,8 +816,14 @@
       <c r="I18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
@@ -724,8 +842,14 @@
       <c r="I19" s="1">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
@@ -744,13 +868,23 @@
       <c r="I20" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
@@ -769,8 +903,11 @@
       <c r="I23" s="1">
         <v>0.95740000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
@@ -789,8 +926,11 @@
       <c r="I24" s="1">
         <v>0.94650000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
@@ -809,6 +949,15 @@
       <c r="I25" s="1">
         <v>0.9476</v>
       </c>
+      <c r="K25" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
temporary fix for metapath2vec dataloader index error
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBC4666-CAA2-49DF-A298-CD25003058AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C45581-4FB0-409A-94DC-71C7074498D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,13 +159,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,10 +189,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,8 +204,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,7 +492,7 @@
   <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +527,7 @@
       <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -535,7 +553,7 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>5</v>
       </c>
       <c r="I4" s="1">
@@ -561,7 +579,7 @@
       <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>6</v>
       </c>
       <c r="I5" s="1">
@@ -587,7 +605,7 @@
       <c r="G6" s="1">
         <v>7</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>7</v>
       </c>
       <c r="I6" s="1">
@@ -613,7 +631,7 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>0.75</v>
       </c>
       <c r="I7" s="1">
@@ -639,7 +657,7 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>1</v>
       </c>
       <c r="I8" s="1">
@@ -665,7 +683,7 @@
       <c r="G9" s="1">
         <v>128</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>64</v>
       </c>
       <c r="I9" s="1">
@@ -679,18 +697,22 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="5"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="5"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H12" s="5"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="5"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -706,7 +728,7 @@
       <c r="G14" s="1">
         <v>256</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>256</v>
       </c>
       <c r="I14" s="1">
@@ -732,7 +754,7 @@
       <c r="G15" s="1">
         <v>256</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>64</v>
       </c>
       <c r="I15" s="1">
@@ -758,7 +780,7 @@
       <c r="G16" s="1">
         <v>200</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>100</v>
       </c>
       <c r="I16" s="1">
@@ -784,7 +806,7 @@
       <c r="G17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I17" t="s">
@@ -810,7 +832,7 @@
       <c r="G18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -836,7 +858,7 @@
       <c r="G19" s="1">
         <v>0.1</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>0.2</v>
       </c>
       <c r="I19" s="1">
@@ -862,7 +884,7 @@
       <c r="G20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>2</v>
       </c>
       <c r="I20" s="1">
@@ -876,12 +898,14 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="H22" s="5"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -897,7 +921,7 @@
       <c r="G23" s="1">
         <v>0.98419999999999996</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <v>0.98250000000000004</v>
       </c>
       <c r="I23" s="1">
@@ -920,7 +944,7 @@
       <c r="G24" s="1">
         <v>0.97699999999999998</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="4">
         <v>0.97440000000000004</v>
       </c>
       <c r="I24" s="1">
@@ -943,7 +967,7 @@
       <c r="G25" s="1">
         <v>0.9758</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
         <v>0.97840000000000005</v>
       </c>
       <c r="I25" s="1">

</xml_diff>

<commit_message>
acquired explanations for g2 params #3
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C45581-4FB0-409A-94DC-71C7074498D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D43C87-F1D1-4E73-9933-15D42A42F851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -145,6 +145,24 @@
   </si>
   <si>
     <t>G2</t>
+  </si>
+  <si>
+    <t>0.003790907945455418</t>
+  </si>
+  <si>
+    <t>0.0818023470545465</t>
+  </si>
+  <si>
+    <t>for G2 with params #3</t>
+  </si>
+  <si>
+    <t>epoch 0</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>epoch 99</t>
   </si>
 </sst>
 </file>
@@ -489,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N27"/>
+  <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,6 +583,9 @@
       <c r="M4" s="1">
         <v>10</v>
       </c>
+      <c r="N4" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
@@ -591,6 +612,9 @@
       <c r="M5" s="1">
         <v>5</v>
       </c>
+      <c r="N5" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
@@ -617,6 +641,9 @@
       <c r="M6" s="1">
         <v>50</v>
       </c>
+      <c r="N6" s="1">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
@@ -643,6 +670,9 @@
       <c r="M7" s="1">
         <v>7</v>
       </c>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
@@ -669,6 +699,9 @@
       <c r="M8" s="1">
         <v>32</v>
       </c>
+      <c r="N8" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
@@ -695,6 +728,9 @@
       <c r="M9" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H10" s="5"/>
@@ -740,6 +776,9 @@
       <c r="M14" s="1">
         <v>64</v>
       </c>
+      <c r="N14" s="1">
+        <v>128</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
@@ -766,6 +805,9 @@
       <c r="M15" s="1">
         <v>64</v>
       </c>
+      <c r="N15" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
@@ -792,8 +834,11 @@
       <c r="M16" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
@@ -818,8 +863,11 @@
       <c r="M17" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
@@ -844,8 +892,11 @@
       <c r="M18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
@@ -870,8 +921,11 @@
       <c r="M19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
@@ -896,19 +950,22 @@
       <c r="M20" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H21" s="5"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="5"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
@@ -931,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
@@ -954,7 +1011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
@@ -977,11 +1034,76 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K27" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="3">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H32" s="3">
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="3">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="3">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enabled counting occurrences of edge/node types for each explanation
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D43C87-F1D1-4E73-9933-15D42A42F851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC24CB60-385B-4B45-AEC0-09AD06DD650F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameter Values" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -163,13 +164,34 @@
   </si>
   <si>
     <t>epoch 99</t>
+  </si>
+  <si>
+    <t>ROC</t>
+  </si>
+  <si>
+    <t>0.9710497611145382</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>0.9087070785403473</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>f1 score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +202,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,6 +256,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -507,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N37"/>
+  <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +554,7 @@
     <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" customWidth="1"/>
     <col min="13" max="13" width="23.5703125" style="1" customWidth="1"/>
@@ -1040,73 +1074,177 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K27" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="3">
-        <v>0.96750000000000003</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H31" s="3">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H32" s="3">
-        <v>0.95069999999999999</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="3">
-        <v>0.97809999999999997</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H36" s="3">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="3">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42147D3A-2308-4FB6-930D-E5A71A6B1B7A}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.96750000000000003</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3">
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="D15">
+        <v>0.85</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.86</v>
+      </c>
+      <c r="D16">
+        <v>0.96</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added legend to explanation graphs
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC24CB60-385B-4B45-AEC0-09AD06DD650F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80F9CFF-70C7-4450-9D72-B1179B32616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Values" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -185,13 +185,37 @@
   </si>
   <si>
     <t>f1 score</t>
+  </si>
+  <si>
+    <t>G1 #1</t>
+  </si>
+  <si>
+    <t>for G1 with params #1</t>
+  </si>
+  <si>
+    <t>epoch 149</t>
+  </si>
+  <si>
+    <t>0.9814351014023793</t>
+  </si>
+  <si>
+    <t>0.9394881607270988</t>
+  </si>
+  <si>
+    <t>for G1 with params previous work</t>
+  </si>
+  <si>
+    <t>0.9758804455316348</t>
+  </si>
+  <si>
+    <t>0.929898731688133</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,8 +238,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +256,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,11 +273,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,10 +296,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,8 +611,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E3" s="1" t="s">
-        <v>8</v>
+      <c r="E3" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -596,7 +637,7 @@
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="7">
         <v>10</v>
       </c>
       <c r="F4" s="1">
@@ -625,7 +666,7 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="7">
         <v>4</v>
       </c>
       <c r="F5" s="1">
@@ -654,7 +695,7 @@
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="7">
         <v>7</v>
       </c>
       <c r="F6" s="1">
@@ -683,7 +724,7 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="7">
         <v>0.75</v>
       </c>
       <c r="F7" s="1">
@@ -712,7 +753,7 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="7">
         <v>0.75</v>
       </c>
       <c r="F8" s="1">
@@ -741,7 +782,7 @@
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="7">
         <v>64</v>
       </c>
       <c r="F9" s="1">
@@ -767,10 +808,12 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10" s="7"/>
       <c r="H10" s="5"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E11" s="7"/>
       <c r="H11" s="5"/>
       <c r="K11" s="2"/>
     </row>
@@ -778,10 +821,12 @@
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E12" s="7"/>
       <c r="H12" s="5"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E13" s="7"/>
       <c r="H13" s="5"/>
       <c r="K13" s="2"/>
     </row>
@@ -789,7 +834,7 @@
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="7">
         <v>64</v>
       </c>
       <c r="F14" s="1">
@@ -818,7 +863,7 @@
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="7">
         <v>128</v>
       </c>
       <c r="F15" s="1">
@@ -847,7 +892,7 @@
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="7">
         <v>150</v>
       </c>
       <c r="F16" s="1">
@@ -876,7 +921,7 @@
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -905,7 +950,7 @@
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -934,7 +979,7 @@
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="7">
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -963,7 +1008,7 @@
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="7">
         <v>2</v>
       </c>
       <c r="F20" s="1">
@@ -989,6 +1034,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E21" s="7"/>
       <c r="H21" s="5"/>
       <c r="K21" s="2"/>
     </row>
@@ -996,6 +1042,7 @@
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="E22" s="7"/>
       <c r="H22" s="5"/>
       <c r="K22" s="2"/>
     </row>
@@ -1003,7 +1050,7 @@
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="7">
         <v>0.99029999999999996</v>
       </c>
       <c r="F23" s="1">
@@ -1026,7 +1073,7 @@
       <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="1">
@@ -1049,7 +1096,7 @@
       <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="7">
         <v>0.98250000000000004</v>
       </c>
       <c r="F25" s="1">
@@ -1082,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42147D3A-2308-4FB6-930D-E5A71A6B1B7A}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,14 +1140,26 @@
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="3" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="1" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>43</v>
       </c>
@@ -1110,8 +1169,26 @@
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.95930000000000004</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0.93810000000000004</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3">
@@ -1120,8 +1197,20 @@
       <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I3" s="3">
+        <v>0.93569999999999998</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3">
@@ -1130,121 +1219,263 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4" s="3">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.98829999999999996</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.99250000000000005</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="3">
-        <v>0.97809999999999997</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.98009999999999997</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.97909999999999997</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3">
-        <v>0.96799999999999997</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.97589999999999999</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="3">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0.95</v>
+      </c>
+      <c r="D14">
+        <v>0.85</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
+        <v>0.86</v>
+      </c>
+      <c r="D15">
+        <v>0.96</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3">
         <v>0.95</v>
       </c>
-      <c r="D15">
-        <v>0.85</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="P15" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0.86</v>
-      </c>
-      <c r="D16">
-        <v>0.96</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0.91</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new explanations generated for g2 e2v
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80F9CFF-70C7-4450-9D72-B1179B32616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9FEC6-79F9-45E0-BC94-03BB7D3F6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Values" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -148,12 +148,6 @@
     <t>G2</t>
   </si>
   <si>
-    <t>0.003790907945455418</t>
-  </si>
-  <si>
-    <t>0.0818023470545465</t>
-  </si>
-  <si>
     <t>for G2 with params #3</t>
   </si>
   <si>
@@ -209,6 +203,15 @@
   </si>
   <si>
     <t>0.929898731688133</t>
+  </si>
+  <si>
+    <t>for G2 with m2v</t>
+  </si>
+  <si>
+    <t>0.010631597403622543</t>
+  </si>
+  <si>
+    <t>0.04801629135272712</t>
   </si>
 </sst>
 </file>
@@ -584,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +615,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>23</v>
@@ -688,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -746,7 +749,7 @@
         <v>7</v>
       </c>
       <c r="N7" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -804,7 +807,7 @@
         <v>36</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -856,7 +859,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="1">
-        <v>128</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -885,7 +888,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="1">
-        <v>64</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -914,7 +917,7 @@
         <v>150</v>
       </c>
       <c r="N16" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -943,7 +946,7 @@
         <v>38</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1001,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1129,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42147D3A-2308-4FB6-930D-E5A71A6B1B7A}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,18 +1153,18 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3">
         <v>0.96750000000000003</v>
@@ -1170,7 +1173,7 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="3">
         <v>0.95930000000000004</v>
@@ -1179,7 +1182,7 @@
         <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O2" s="3">
         <v>0.93810000000000004</v>
@@ -1195,19 +1198,19 @@
         <v>0.94799999999999995</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3" s="3">
         <v>0.93569999999999998</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O3" s="3">
         <v>0.91600000000000004</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1241,7 +1244,7 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3">
         <v>0.97809999999999997</v>
@@ -1250,7 +1253,7 @@
         <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I6" s="3">
         <v>0.98829999999999996</v>
@@ -1259,7 +1262,7 @@
         <v>16</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O6" s="3">
         <v>0.99250000000000005</v>
@@ -1275,19 +1278,19 @@
         <v>0.96799999999999997</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="3">
         <v>0.98009999999999997</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O7" s="3">
         <v>0.97909999999999997</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1319,43 +1322,43 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1366,31 +1369,31 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
       <c r="I13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" t="s">
         <v>50</v>
       </c>
-      <c r="J13" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" t="s">
-        <v>52</v>
-      </c>
       <c r="O13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1473,6 +1476,11 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more explanations generated for g1 and e2v
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB9FEC6-79F9-45E0-BC94-03BB7D3F6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAC80CA-59E8-4F68-B2B3-722E9A0D0D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4680" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Values" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -211,14 +211,53 @@
     <t>0.010631597403622543</t>
   </si>
   <si>
-    <t>0.04801629135272712</t>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>weight decay</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.7968</t>
+  </si>
+  <si>
+    <t>0.7805</t>
+  </si>
+  <si>
+    <t>0.7734</t>
+  </si>
+  <si>
+    <t>0.9789</t>
+  </si>
+  <si>
+    <t>0.9098</t>
+  </si>
+  <si>
+    <t>0.9109</t>
+  </si>
+  <si>
+    <t>G1 PREV</t>
+  </si>
+  <si>
+    <t>with 3 explanations</t>
+  </si>
+  <si>
+    <t>0.9786370457263286</t>
+  </si>
+  <si>
+    <t>0.933313705284852</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,15 +280,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,11 +291,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,10 +303,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -299,14 +325,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,62 +610,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:N27"/>
+  <dimension ref="A2:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="27.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E3" s="7" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>10</v>
       </c>
       <c r="F4" s="1">
@@ -649,56 +678,62 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4">
         <v>5</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>10</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>10</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
         <v>4</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="4">
         <v>6</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>6</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>5</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>7</v>
       </c>
       <c r="F6" s="1">
@@ -707,253 +742,277 @@
       <c r="G6" s="1">
         <v>7</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>7</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>50</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.75</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
         <v>0.75</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>0.5</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="M7" s="1">
-        <v>7</v>
       </c>
       <c r="N7" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.75</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="4">
         <v>1</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>32</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7">
-        <v>64</v>
+      <c r="E9" s="4">
+        <v>32</v>
       </c>
       <c r="F9" s="1">
         <v>64</v>
       </c>
       <c r="G9" s="1">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1">
         <v>128</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>64</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>64</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E10" s="7"/>
-      <c r="H10" s="5"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="7"/>
-      <c r="H11" s="5"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="H12" s="5"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="I13" s="5"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
+        <v>256</v>
+      </c>
+      <c r="F14" s="1">
         <v>64</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>128</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>256</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>256</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>64</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>64</v>
       </c>
-      <c r="N14" s="1">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1">
         <v>128</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>64</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>256</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>64</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>64</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>64</v>
       </c>
-      <c r="N15" s="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>150</v>
       </c>
       <c r="F16" s="1">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G16" s="1">
         <v>200</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="1">
+        <v>200</v>
+      </c>
+      <c r="I16" s="4">
         <v>100</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>150</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="M16" s="1">
-        <v>150</v>
       </c>
       <c r="N16" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -962,167 +1021,184 @@
       <c r="G18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>0.2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>0.1</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <v>0.2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>0.1</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="M19" s="1">
-        <v>0</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>2</v>
       </c>
       <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
         <v>4</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="4">
+      <c r="I20" s="4">
         <v>2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>2</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="M20" s="1">
-        <v>6</v>
       </c>
       <c r="N20" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E21" s="7"/>
-      <c r="H21" s="5"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="I21" s="5"/>
+      <c r="L21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="H22" s="5"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="I22" s="5"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4"/>
+      <c r="F23" s="1">
         <v>0.99029999999999996</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>0.98750000000000004</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>0.98419999999999996</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <v>0.98250000000000004</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>0.95740000000000003</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>0.96150000000000002</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>0.97699999999999998</v>
       </c>
-      <c r="H24" s="4">
+      <c r="I24" s="4">
         <v>0.97440000000000004</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>0.94650000000000001</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4"/>
+      <c r="F25" s="1">
         <v>0.98250000000000004</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>0.96419999999999995</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>0.9758</v>
       </c>
-      <c r="H25" s="4">
+      <c r="I25" s="4">
         <v>0.97840000000000005</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>0.9476</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K27" s="2"/>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1132,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42147D3A-2308-4FB6-930D-E5A71A6B1B7A}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1234,7 @@
       <c r="G1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1180,6 +1256,9 @@
       </c>
       <c r="J2" t="s">
         <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>41</v>
@@ -1477,9 +1556,248 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0.93720000000000003</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M21" s="5"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="8">
+        <v>0.90269999999999995</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="8">
+        <v>0.97870000000000001</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M25" s="5"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="8">
+        <v>0.97860000000000003</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0.9</v>
+      </c>
+      <c r="D27">
+        <v>0.63</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.72</v>
+      </c>
+      <c r="D28">
+        <v>0.93</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M30" s="5"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M31" s="5"/>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M32" s="5"/>
+      <c r="N32" s="4">
+        <v>1</v>
+      </c>
+      <c r="O32" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="P32" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>0.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
looking at variability of edge2vec embedding
</commit_message>
<xml_diff>
--- a/output/hyperparameter_optimization_results.xlsx
+++ b/output/hyperparameter_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosa-\Google Drive\Msc_Bioinformatics\thesis\XAIFO-ThesisProject\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAC80CA-59E8-4F68-B2B3-722E9A0D0D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3797D0B-9A8F-4A6C-B404-B3F213A42369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7485" yWindow="-10275" windowWidth="15090" windowHeight="9930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Values" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="93">
   <si>
     <t>NODE EMBEDDING</t>
   </si>
@@ -251,13 +251,67 @@
   </si>
   <si>
     <t>0.933313705284852</t>
+  </si>
+  <si>
+    <t>for G2 with params #3 alternative</t>
+  </si>
+  <si>
+    <t>0.9664</t>
+  </si>
+  <si>
+    <t>0.9354</t>
+  </si>
+  <si>
+    <t>0.9353</t>
+  </si>
+  <si>
+    <t>0.9785</t>
+  </si>
+  <si>
+    <t>0.9669</t>
+  </si>
+  <si>
+    <t>0.9734</t>
+  </si>
+  <si>
+    <t>0.9733971388937009</t>
+  </si>
+  <si>
+    <t>0.91288746703558</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>with 19 explanations</t>
+  </si>
+  <si>
+    <t>with 10 explanations</t>
+  </si>
+  <si>
+    <t>with 14 explanations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +330,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,11 +373,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,8 +400,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -612,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="69" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1210,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42147D3A-2308-4FB6-930D-E5A71A6B1B7A}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="67" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1299,7 @@
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="3" customWidth="1"/>
     <col min="13" max="13" width="31.42578125" customWidth="1"/>
@@ -1231,14 +1311,21 @@
       <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>52</v>
       </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
       <c r="M1" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1248,16 +1335,18 @@
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="11">
         <v>0.95930000000000004</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="K2" s="12"/>
+      <c r="M2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -1279,12 +1368,15 @@
       <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="3">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11">
         <v>0.93569999999999998</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="K3" s="12"/>
       <c r="O3" s="3">
         <v>0.91600000000000004</v>
       </c>
@@ -1301,12 +1393,15 @@
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="3">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11">
         <v>0.93389999999999995</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="K4" s="12"/>
       <c r="O4" s="3">
         <v>0.91720000000000002</v>
       </c>
@@ -1319,6 +1414,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1331,15 +1431,17 @@
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="11">
         <v>0.98829999999999996</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="K6" s="12"/>
       <c r="N6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1359,12 +1461,15 @@
       <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="3">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11">
         <v>0.98009999999999997</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="12" t="s">
         <v>42</v>
       </c>
+      <c r="K7" s="12"/>
       <c r="O7" s="3">
         <v>0.97909999999999997</v>
       </c>
@@ -1381,12 +1486,15 @@
       <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="3">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11">
         <v>0.98140000000000005</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="K8" s="12"/>
       <c r="O8" s="3">
         <v>0.97589999999999999</v>
       </c>
@@ -1397,6 +1505,11 @@
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1406,12 +1519,15 @@
       <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="N10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1427,12 +1543,15 @@
       <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="11" t="s">
         <v>55</v>
       </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="N11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1443,6 +1562,11 @@
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -1456,13 +1580,15 @@
       <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="12" t="s">
         <v>50</v>
       </c>
       <c r="O13" s="3" t="s">
@@ -1489,16 +1615,17 @@
       <c r="E14" s="1">
         <v>0.9</v>
       </c>
-      <c r="H14" s="1">
+      <c r="G14" s="10"/>
+      <c r="H14" s="10">
         <v>0</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="11">
         <v>0.94</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="10">
         <v>0.93</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="10">
         <v>0.94</v>
       </c>
       <c r="N14" s="1">
@@ -1528,16 +1655,17 @@
       <c r="E15" s="1">
         <v>0.91</v>
       </c>
-      <c r="H15" s="1">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10">
         <v>1</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="11">
         <v>0.94</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="10">
         <v>0.94</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="10">
         <v>0.94</v>
       </c>
       <c r="N15" s="1">
@@ -1569,7 +1697,10 @@
       <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="G18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="9" t="s">
         <v>56</v>
       </c>
       <c r="N18" s="4"/>
@@ -1584,7 +1715,21 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="5"/>
+      <c r="G19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="N19" s="4" t="s">
         <v>41</v>
       </c>
@@ -1602,6 +1747,12 @@
       </c>
       <c r="D20" t="s">
         <v>17</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="4"/>
@@ -1614,6 +1765,12 @@
       <c r="Q20" s="8"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M21" s="5"/>
       <c r="N21" s="4"/>
       <c r="O21" s="8">
@@ -1634,6 +1791,7 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
+      <c r="J22" s="3"/>
       <c r="M22" s="5"/>
       <c r="N22" s="4"/>
       <c r="O22" s="8"/>
@@ -1647,6 +1805,15 @@
       <c r="D23" t="s">
         <v>42</v>
       </c>
+      <c r="H23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="M23" s="5"/>
       <c r="N23" s="4" t="s">
         <v>53</v>
@@ -1665,6 +1832,12 @@
       </c>
       <c r="D24" t="s">
         <v>17</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="4"/>
@@ -1677,6 +1850,12 @@
       <c r="Q24" s="8"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M25" s="5"/>
       <c r="N25" s="4"/>
       <c r="O25" s="8">
@@ -1717,6 +1896,12 @@
       <c r="E27" s="1">
         <v>0.74</v>
       </c>
+      <c r="H27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="M27" s="5"/>
       <c r="N27" s="4" t="s">
         <v>44</v>
@@ -1739,6 +1924,12 @@
       </c>
       <c r="E28" s="1">
         <v>0.81</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="4" t="s">
@@ -1758,6 +1949,15 @@
       <c r="Q29" s="8"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" t="s">
+        <v>49</v>
+      </c>
+      <c r="K30" t="s">
+        <v>50</v>
+      </c>
       <c r="M30" s="5"/>
       <c r="N30" s="4"/>
       <c r="O30" s="8" t="s">
@@ -1771,6 +1971,18 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J31" t="s">
+        <v>85</v>
+      </c>
+      <c r="K31" t="s">
+        <v>86</v>
+      </c>
       <c r="M31" s="5"/>
       <c r="N31" s="4">
         <v>0</v>
@@ -1786,6 +1998,18 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" t="s">
+        <v>89</v>
+      </c>
       <c r="M32" s="5"/>
       <c r="N32" s="4">
         <v>1</v>

</xml_diff>